<commit_message>
added some additional analysis
</commit_message>
<xml_diff>
--- a/Data/novel_component_elbow_loc_sens.xlsx
+++ b/Data/novel_component_elbow_loc_sens.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erezfreud/Documents/Shape_Sensitivity_LifeSpan/Analyzed/Shape_Sensetivity_LifeSpan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jenn\Documents\ShapeSensitivity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF7657C-2EB8-49B4-8F83-C818AACA0BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" tabRatio="500"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="16005" windowHeight="10860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="18">
   <si>
     <t>ventral_right</t>
   </si>
@@ -64,11 +73,29 @@
   <si>
     <t>Dorsal_left</t>
   </si>
+  <si>
+    <t>Pathway</t>
+  </si>
+  <si>
+    <t>Hemi</t>
+  </si>
+  <si>
+    <t>ventral</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>dorsal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,12 +137,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -154,7 +184,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -231,20 +260,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23022815585541</c:v>
+                  <c:v>0.23022815585541048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.180088314649256</c:v>
+                  <c:v>0.18008831464925587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0307252960032165</c:v>
+                  <c:v>-3.0725296003216506E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0533761268283675</c:v>
+                  <c:v>-5.337612682836753E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49E7-4E06-9AE5-35048047CB93}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -332,6 +366,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -412,7 +447,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -456,7 +491,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -533,20 +567,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.122028241964537</c:v>
+                  <c:v>0.12202824196453736</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.132008985298707</c:v>
+                  <c:v>0.13200898529870733</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.111005007849507</c:v>
+                  <c:v>0.11100500784950718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.08914533116618</c:v>
+                  <c:v>8.914533116618005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99A9-4938-8DDE-3B11401C9901}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -617,7 +656,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -635,6 +674,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1819,7 +1859,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1849,7 +1895,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2129,20 +2181,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2161,8 +2214,14 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2181,8 +2240,14 @@
       <c r="F2">
         <v>0.25302957651066399</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2201,8 +2266,14 @@
       <c r="F3">
         <v>0.272948996324476</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2221,6 +2292,12 @@
       <c r="F4">
         <v>0.42683435964218702</v>
       </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
@@ -2246,7 +2323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2264,6 +2341,12 @@
       </c>
       <c r="F5">
         <v>0.175404363516002</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
       </c>
       <c r="I5">
         <f>AVERAGE(F2:F13)</f>
@@ -2298,7 +2381,7 @@
         <v>8.914533116618005E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2317,8 +2400,14 @@
       <c r="F6">
         <v>-3.51602917779376E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2337,8 +2426,14 @@
       <c r="F7">
         <v>0.226813574031168</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2357,8 +2452,14 @@
       <c r="F8">
         <v>0.175718802402795</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2377,8 +2478,14 @@
       <c r="F9">
         <v>0.227267089934373</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2397,8 +2504,14 @@
       <c r="F10">
         <v>0.21644130269602599</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -2417,8 +2530,14 @@
       <c r="F11">
         <v>0.21764296940507999</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2437,8 +2556,14 @@
       <c r="F12">
         <v>0.22092674073115301</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -2457,8 +2582,14 @@
       <c r="F13">
         <v>0.38487038684893998</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -2477,8 +2608,14 @@
       <c r="F14">
         <v>0.233177215578763</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -2497,8 +2634,14 @@
       <c r="F15">
         <v>7.3869327447898897E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -2517,8 +2660,14 @@
       <c r="F16">
         <v>0.31367768099305199</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2537,8 +2686,14 @@
       <c r="F17">
         <v>9.2733390014389003E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2557,8 +2712,14 @@
       <c r="F18">
         <v>0.17228788841915699</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2577,8 +2738,14 @@
       <c r="F19">
         <v>0.17626663687430699</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2597,8 +2764,14 @@
       <c r="F20">
         <v>0.271106590881461</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2617,8 +2790,14 @@
       <c r="F21">
         <v>-8.4551613760909805E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2637,8 +2816,14 @@
       <c r="F22">
         <v>0.245726335050411</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2657,8 +2842,14 @@
       <c r="F23">
         <v>0.208161891099475</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2677,8 +2868,14 @@
       <c r="F24">
         <v>0.19250534799176899</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2697,8 +2894,14 @@
       <c r="F25">
         <v>0.26609908520129699</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2717,8 +2920,14 @@
       <c r="F26">
         <v>5.1801262394073604E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2737,8 +2946,14 @@
       <c r="F27">
         <v>0.28761046956298197</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2757,8 +2972,14 @@
       <c r="F28">
         <v>5.9525940857012703E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2777,8 +2998,14 @@
       <c r="F29">
         <v>3.1720534554231197E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2797,8 +3024,14 @@
       <c r="F30">
         <v>-0.29321248496683999</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2817,8 +3050,14 @@
       <c r="F31">
         <v>-0.10475455031325499</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -2837,8 +3076,14 @@
       <c r="F32">
         <v>3.0785904998961301E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -2857,8 +3102,14 @@
       <c r="F33">
         <v>-7.4719859399918404E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -2877,8 +3128,14 @@
       <c r="F34">
         <v>0.14221055412191599</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -2897,8 +3154,14 @@
       <c r="F35">
         <v>0.10362904757508</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -2917,8 +3180,14 @@
       <c r="F36">
         <v>-0.102970571071372</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -2937,8 +3206,14 @@
       <c r="F37">
         <v>-0.42600134969773801</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0</v>
       </c>
@@ -2957,8 +3232,14 @@
       <c r="F38">
         <v>-4.2308338208507396E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2977,8 +3258,14 @@
       <c r="F39">
         <v>0.12278800680924</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -2997,8 +3284,14 @@
       <c r="F40">
         <v>0.19086519841857599</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -3017,8 +3310,14 @@
       <c r="F41">
         <v>-0.12953940087049601</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -3037,8 +3336,14 @@
       <c r="F42">
         <v>-0.126446374991486</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -3057,8 +3362,14 @@
       <c r="F43">
         <v>0.21054485287960001</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -3077,8 +3388,14 @@
       <c r="F44">
         <v>-0.33723362563810899</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0</v>
       </c>
@@ -3097,8 +3414,14 @@
       <c r="F45">
         <v>-0.29465734006554101</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0</v>
       </c>
@@ -3117,8 +3440,14 @@
       <c r="F46">
         <v>4.4698160301004002E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -3137,8 +3466,14 @@
       <c r="F47">
         <v>-0.114891957869828</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
@@ -3157,8 +3492,14 @@
       <c r="F48">
         <v>7.7194769644044106E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0</v>
       </c>
@@ -3176,6 +3517,12 @@
       </c>
       <c r="F49">
         <v>-0.23937663246565999</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>